<commit_message>
save modified video added
</commit_message>
<xml_diff>
--- a/python/VIY/data_summary.xlsx
+++ b/python/VIY/data_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,14 +473,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -499,21 +499,99 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>50</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>6-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>29/05/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>57</v>
+      </c>
+      <c r="D4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>15-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>29/05/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>44</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>15-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>29/05/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>78</v>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6-14</t>
         </is>
       </c>
     </row>

</xml_diff>